<commit_message>
clickmeter data & tracking reports & pdf
</commit_message>
<xml_diff>
--- a/ADSDataDirect.Web/Templates/Tracking3.xlsx
+++ b/ADSDataDirect.Web/Templates/Tracking3.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ADSDataDirect\ADSDataDirect.Web\Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="11688"/>
   </bookViews>
@@ -23,7 +28,7 @@
     <definedName name="Day_MM">INDIRECT([1]Output!#REF!)</definedName>
     <definedName name="White_Label">INDIRECT([1]Output!$B$9)</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>Total Opens</t>
   </si>
@@ -60,9 +65,6 @@
     <t>Clicks to opens</t>
   </si>
   <si>
-    <t>Key statistics for this compaign:</t>
-  </si>
-  <si>
     <t>Send time:</t>
   </si>
   <si>
@@ -120,17 +122,17 @@
     <t>Unsubscribe</t>
   </si>
   <si>
-    <t>Unsub to opens</t>
+    <t>Key statistics for this campaign:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,14 +181,6 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -328,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -344,9 +338,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -357,12 +351,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -373,7 +367,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -381,80 +375,77 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="17" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="16" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -528,7 +519,7 @@
         <xdr:cNvPr id="5" name="Rectangle: Rounded Corners 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -599,7 +590,7 @@
         <xdr:cNvPr id="6" name="Rectangle: Rounded Corners 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -670,7 +661,7 @@
         <xdr:cNvPr id="7" name="Rectangle: Rounded Corners 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -739,7 +730,7 @@
         <xdr:cNvPr id="10" name="Straight Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -796,7 +787,7 @@
         <xdr:cNvPr id="13" name="Straight Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -853,7 +844,7 @@
         <xdr:cNvPr id="14" name="Straight Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -896,21 +887,21 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>165735</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>558165</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>154305</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="19" name="Rectangle: Rounded Corners 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B8D8E01-52D6-4552-90F5-7E14FF82D50B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2B8D8E01-52D6-4552-90F5-7E14FF82D50B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -918,7 +909,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7620" y="5857875"/>
+          <a:off x="7620" y="5339715"/>
           <a:ext cx="1160145" cy="361950"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -961,137 +952,11 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>165734</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>558165</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>158114</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="Rectangle: Rounded Corners 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{830D2B11-B885-4748-BF82-F6A1BC0361D3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7620" y="5293994"/>
-          <a:ext cx="1160145" cy="365760"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="7030A0"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" b="1"/>
-            <a:t>Shared</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>5716</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1188720</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="22" name="Straight Connector 21">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0112EFA-085C-4A85-AEB6-0B89CEB7245F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5716" y="5760720"/>
-          <a:ext cx="7720964" cy="30480"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Orders"/>
@@ -1416,22 +1281,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="4" width="11.6640625" customWidth="1"/>
     <col min="5" max="5" width="4.33203125" customWidth="1"/>
@@ -1446,41 +1311,41 @@
     <col min="14" max="14" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1">
-      <c r="A1" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
       <c r="J1" s="23"/>
       <c r="K1" s="23"/>
       <c r="L1" s="23"/>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
       <c r="J2" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="23"/>
       <c r="L2" s="26">
         <v>43041</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="1.2" customHeight="1">
+    <row r="3" spans="1:12" ht="1.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22"/>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
@@ -1494,7 +1359,7 @@
       <c r="K3" s="22"/>
       <c r="L3" s="22"/>
     </row>
-    <row r="4" spans="1:12" ht="1.2" customHeight="1">
+    <row r="4" spans="1:12" ht="1.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22"/>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
@@ -1508,7 +1373,7 @@
       <c r="K4" s="22"/>
       <c r="L4" s="22"/>
     </row>
-    <row r="5" spans="1:12" ht="1.2" customHeight="1">
+    <row r="5" spans="1:12" ht="1.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22"/>
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
@@ -1522,152 +1387,152 @@
       <c r="K5" s="22"/>
       <c r="L5" s="22"/>
     </row>
-    <row r="6" spans="1:12" ht="21.6" customHeight="1">
+    <row r="6" spans="1:12" ht="21.6" customHeight="1" x14ac:dyDescent="0.6">
       <c r="D6" s="10"/>
-      <c r="H6" s="31"/>
+      <c r="H6" s="49"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="44" t="s">
+      <c r="J6" s="37" t="s">
         <v>3</v>
       </c>
       <c r="K6" s="5"/>
-      <c r="L6" s="32">
+      <c r="L6" s="50">
         <v>50000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1">
-      <c r="H7" s="31"/>
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="49"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="44"/>
+      <c r="J7" s="37"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="32"/>
-    </row>
-    <row r="8" spans="1:12" ht="14.4" customHeight="1">
+      <c r="L7" s="50"/>
+    </row>
+    <row r="8" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H8" s="6"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="45" t="s">
+      <c r="J8" s="38" t="s">
         <v>4</v>
       </c>
       <c r="K8" s="7"/>
-      <c r="L8" s="37">
+      <c r="L8" s="42">
         <f>H26/C23</f>
         <v>0.11650000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="14.4" customHeight="1">
+    <row r="9" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H9" s="6"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="45"/>
+      <c r="J9" s="38"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="37"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A10" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="30"/>
+      <c r="L9" s="42"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="48"/>
       <c r="C10" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="31"/>
+      <c r="H10" s="49"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="46" t="s">
+      <c r="J10" s="39" t="s">
         <v>5</v>
       </c>
       <c r="K10" s="8"/>
-      <c r="L10" s="43">
+      <c r="L10" s="46">
         <f>H29/C23</f>
         <v>2.1659999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.6">
-      <c r="A11" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="30"/>
+    <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="48"/>
       <c r="C11" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
-      <c r="H11" s="31"/>
+      <c r="H11" s="49"/>
       <c r="I11" s="8"/>
-      <c r="J11" s="46"/>
+      <c r="J11" s="39"/>
       <c r="K11" s="8"/>
-      <c r="L11" s="43"/>
-    </row>
-    <row r="12" spans="1:12" ht="7.8" hidden="1" customHeight="1">
+      <c r="L11" s="46"/>
+    </row>
+    <row r="12" spans="1:12" ht="7.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="C12" s="15"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A13" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="30"/>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="48"/>
       <c r="C13" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="39"/>
+      <c r="H13" s="44"/>
       <c r="I13" s="27"/>
-      <c r="J13" s="48" t="s">
-        <v>26</v>
+      <c r="J13" s="40" t="s">
+        <v>25</v>
       </c>
       <c r="K13" s="27"/>
-      <c r="L13" s="50">
-        <f>H35/C23</f>
+      <c r="L13" s="28">
+        <f>H32/C23</f>
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A14" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="30"/>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="48"/>
       <c r="C14" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="39"/>
+      <c r="H14" s="44"/>
       <c r="I14" s="27"/>
-      <c r="J14" s="48"/>
+      <c r="J14" s="40"/>
       <c r="K14" s="27"/>
-      <c r="L14" s="50"/>
-    </row>
-    <row r="15" spans="1:12" ht="7.5" customHeight="1">
+      <c r="L14" s="28"/>
+    </row>
+    <row r="15" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="C15" s="15"/>
       <c r="H15" s="6"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A16" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="30"/>
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="48"/>
       <c r="C16" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="21"/>
       <c r="I16" s="24"/>
-      <c r="J16" s="36"/>
+      <c r="J16" s="41"/>
       <c r="K16" s="24"/>
-      <c r="L16" s="33"/>
-    </row>
-    <row r="17" spans="1:12" ht="15" customHeight="1">
-      <c r="A17" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="30"/>
+      <c r="L16" s="51"/>
+    </row>
+    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="48"/>
       <c r="C17" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
@@ -1675,15 +1540,15 @@
       <c r="G17" s="29"/>
       <c r="H17" s="29"/>
       <c r="I17" s="24"/>
-      <c r="J17" s="36"/>
+      <c r="J17" s="41"/>
       <c r="K17" s="24"/>
-      <c r="L17" s="33"/>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A18" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="30"/>
+      <c r="L17" s="51"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="48"/>
       <c r="C18" s="20"/>
       <c r="D18" s="29"/>
       <c r="E18" s="29"/>
@@ -1695,9 +1560,9 @@
       <c r="K18" s="29"/>
       <c r="L18" s="29"/>
     </row>
-    <row r="19" spans="1:12" ht="15.6">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
+    <row r="19" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="48"/>
+      <c r="B19" s="48"/>
       <c r="C19" s="20"/>
       <c r="D19" s="29"/>
       <c r="E19" s="29"/>
@@ -1709,7 +1574,7 @@
       <c r="K19" s="29"/>
       <c r="L19" s="29"/>
     </row>
-    <row r="20" spans="1:12" ht="15.6">
+    <row r="20" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="20"/>
@@ -1723,7 +1588,7 @@
       <c r="K20" s="29"/>
       <c r="L20" s="29"/>
     </row>
-    <row r="21" spans="1:12" ht="15.6">
+    <row r="21" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="20"/>
@@ -1737,133 +1602,124 @@
       <c r="K21" s="29"/>
       <c r="L21" s="29"/>
     </row>
-    <row r="22" spans="1:12" ht="23.4">
+    <row r="22" spans="1:12" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="15" customHeight="1">
-      <c r="C23" s="38">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="43">
         <v>50000</v>
       </c>
-      <c r="D23" s="38"/>
+      <c r="D23" s="43"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="41"/>
-      <c r="H23" s="34"/>
+      <c r="F23" s="32"/>
+      <c r="H23" s="36"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="41"/>
-      <c r="L23" s="34"/>
-    </row>
-    <row r="24" spans="1:12" ht="15" customHeight="1">
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
+      <c r="J23" s="32"/>
+      <c r="L23" s="36"/>
+    </row>
+    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="41"/>
-      <c r="H24" s="34"/>
+      <c r="F24" s="32"/>
+      <c r="H24" s="36"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="41"/>
-      <c r="L24" s="34"/>
-    </row>
-    <row r="26" spans="1:12" ht="15" customHeight="1">
-      <c r="C26" s="40">
+      <c r="J24" s="32"/>
+      <c r="L24" s="36"/>
+    </row>
+    <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="33">
         <f>H26/C23</f>
         <v>0.11650000000000001</v>
       </c>
-      <c r="D26" s="42"/>
+      <c r="D26" s="45"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="41" t="s">
+      <c r="F26" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="H26" s="38">
+      <c r="H26" s="43">
         <v>5825</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15" customHeight="1">
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
+    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="41"/>
-      <c r="H27" s="38"/>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="F27" s="32"/>
+      <c r="H27" s="43"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
     </row>
-    <row r="29" spans="1:12" ht="15" customHeight="1">
-      <c r="C29" s="40">
+    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="33">
         <f>H29/C23</f>
         <v>2.1659999999999999E-2</v>
       </c>
-      <c r="D29" s="42"/>
+      <c r="D29" s="45"/>
       <c r="E29" s="4"/>
-      <c r="F29" s="41" t="s">
+      <c r="F29" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="H29" s="38">
+      <c r="H29" s="43">
         <v>1083</v>
       </c>
-      <c r="J29" s="47" t="s">
+      <c r="J29" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="L29" s="40">
+      <c r="L29" s="33">
         <f>H29/H26</f>
         <v>0.18592274678111587</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15" customHeight="1">
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
+    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
       <c r="E30" s="4"/>
-      <c r="F30" s="41"/>
-      <c r="H30" s="38"/>
-      <c r="J30" s="47"/>
-      <c r="L30" s="40"/>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="F30" s="32"/>
+      <c r="H30" s="43"/>
+      <c r="J30" s="34"/>
+      <c r="L30" s="33"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
     </row>
-    <row r="32" spans="1:12" ht="15" customHeight="1">
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
+    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="30">
+        <f>H32/C23</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D32" s="31"/>
       <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="1:12" ht="15" customHeight="1">
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
+      <c r="F32" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="H32" s="35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
       <c r="E33" s="4"/>
-    </row>
-    <row r="35" spans="1:12" ht="15" customHeight="1">
-      <c r="C35" s="51">
-        <f>H35/C23</f>
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="D35" s="52"/>
+      <c r="F33" s="32"/>
+      <c r="H33" s="36"/>
+    </row>
+    <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E35" s="4"/>
-      <c r="F35" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="H35" s="49">
-        <v>25</v>
-      </c>
-      <c r="J35" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="L35" s="40">
-        <f>H35/H26</f>
-        <v>4.2918454935622317E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="15" customHeight="1">
-      <c r="C36" s="52"/>
-      <c r="D36" s="52"/>
+      <c r="J35" s="34"/>
+      <c r="L35" s="33"/>
+    </row>
+    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E36" s="4"/>
-      <c r="F36" s="41"/>
-      <c r="H36" s="34"/>
-      <c r="J36" s="47"/>
-      <c r="L36" s="40"/>
-    </row>
-    <row r="38" spans="1:12" ht="25.95" customHeight="1">
+      <c r="J36" s="34"/>
+      <c r="L36" s="33"/>
+    </row>
+    <row r="38" spans="1:12" ht="25.95" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A38" s="17" t="s">
         <v>1</v>
       </c>
@@ -1881,9 +1737,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="39" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B39" s="29"/>
       <c r="C39" s="29"/>
@@ -1899,9 +1755,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="40" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B40" s="29"/>
       <c r="C40" s="29"/>
@@ -1917,7 +1773,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="41" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="29"/>
       <c r="B41" s="29"/>
       <c r="C41" s="29"/>
@@ -1931,7 +1787,7 @@
       <c r="K41" s="29"/>
       <c r="L41" s="25"/>
     </row>
-    <row r="42" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="42" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="29"/>
       <c r="B42" s="29"/>
       <c r="C42" s="29"/>
@@ -1945,7 +1801,7 @@
       <c r="K42" s="29"/>
       <c r="L42" s="25"/>
     </row>
-    <row r="43" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="43" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="29"/>
       <c r="B43" s="29"/>
       <c r="C43" s="29"/>
@@ -1959,7 +1815,7 @@
       <c r="K43" s="29"/>
       <c r="L43" s="25"/>
     </row>
-    <row r="44" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="44" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="29"/>
       <c r="B44" s="29"/>
       <c r="C44" s="29"/>
@@ -1973,7 +1829,7 @@
       <c r="K44" s="29"/>
       <c r="L44" s="25"/>
     </row>
-    <row r="45" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="45" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="29"/>
       <c r="B45" s="29"/>
       <c r="C45" s="29"/>
@@ -1987,7 +1843,7 @@
       <c r="K45" s="29"/>
       <c r="L45" s="25"/>
     </row>
-    <row r="46" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="46" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="29"/>
       <c r="B46" s="29"/>
       <c r="C46" s="29"/>
@@ -2001,7 +1857,7 @@
       <c r="K46" s="29"/>
       <c r="L46" s="25"/>
     </row>
-    <row r="47" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="47" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="29"/>
       <c r="B47" s="29"/>
       <c r="C47" s="29"/>
@@ -2015,7 +1871,7 @@
       <c r="K47" s="29"/>
       <c r="L47" s="25"/>
     </row>
-    <row r="48" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="48" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="29"/>
       <c r="B48" s="29"/>
       <c r="C48" s="29"/>
@@ -2029,7 +1885,7 @@
       <c r="K48" s="29"/>
       <c r="L48" s="25"/>
     </row>
-    <row r="49" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="49" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="29"/>
       <c r="B49" s="29"/>
       <c r="C49" s="29"/>
@@ -2043,7 +1899,7 @@
       <c r="K49" s="29"/>
       <c r="L49" s="25"/>
     </row>
-    <row r="50" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="50" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="29"/>
       <c r="B50" s="29"/>
       <c r="C50" s="29"/>
@@ -2057,7 +1913,7 @@
       <c r="K50" s="29"/>
       <c r="L50" s="25"/>
     </row>
-    <row r="51" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="51" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="29"/>
       <c r="B51" s="29"/>
       <c r="C51" s="29"/>
@@ -2071,7 +1927,7 @@
       <c r="K51" s="29"/>
       <c r="L51" s="25"/>
     </row>
-    <row r="52" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="52" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="29"/>
       <c r="B52" s="29"/>
       <c r="C52" s="29"/>
@@ -2085,7 +1941,7 @@
       <c r="K52" s="29"/>
       <c r="L52" s="25"/>
     </row>
-    <row r="53" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="53" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="29"/>
       <c r="B53" s="29"/>
       <c r="C53" s="29"/>
@@ -2099,7 +1955,7 @@
       <c r="K53" s="29"/>
       <c r="L53" s="25"/>
     </row>
-    <row r="54" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="54" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="29"/>
       <c r="B54" s="29"/>
       <c r="C54" s="29"/>
@@ -2113,7 +1969,7 @@
       <c r="K54" s="29"/>
       <c r="L54" s="25"/>
     </row>
-    <row r="55" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="55" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="29"/>
       <c r="B55" s="29"/>
       <c r="C55" s="29"/>
@@ -2127,7 +1983,7 @@
       <c r="K55" s="29"/>
       <c r="L55" s="25"/>
     </row>
-    <row r="56" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="56" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="29"/>
       <c r="B56" s="29"/>
       <c r="C56" s="29"/>
@@ -2141,7 +1997,7 @@
       <c r="K56" s="29"/>
       <c r="L56" s="25"/>
     </row>
-    <row r="57" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="57" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="29"/>
       <c r="B57" s="29"/>
       <c r="C57" s="29"/>
@@ -2154,10 +2010,10 @@
       <c r="J57" s="29"/>
       <c r="K57" s="29"/>
       <c r="L57" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="29"/>
       <c r="B58" s="29"/>
       <c r="C58" s="29"/>
@@ -2170,10 +2026,10 @@
       <c r="J58" s="29"/>
       <c r="K58" s="29"/>
       <c r="L58" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="29"/>
       <c r="B59" s="29"/>
       <c r="C59" s="29"/>
@@ -2186,10 +2042,10 @@
       <c r="J59" s="29"/>
       <c r="K59" s="29"/>
       <c r="L59" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="29"/>
       <c r="B60" s="29"/>
       <c r="C60" s="29"/>
@@ -2202,10 +2058,10 @@
       <c r="J60" s="29"/>
       <c r="K60" s="29"/>
       <c r="L60" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="29"/>
       <c r="B61" s="29"/>
       <c r="C61" s="29"/>
@@ -2218,10 +2074,10 @@
       <c r="J61" s="29"/>
       <c r="K61" s="29"/>
       <c r="L61" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="29"/>
       <c r="B62" s="29"/>
       <c r="C62" s="29"/>
@@ -2234,10 +2090,10 @@
       <c r="J62" s="29"/>
       <c r="K62" s="29"/>
       <c r="L62" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="29"/>
       <c r="B63" s="29"/>
       <c r="C63" s="29"/>
@@ -2250,10 +2106,10 @@
       <c r="J63" s="29"/>
       <c r="K63" s="29"/>
       <c r="L63" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="29"/>
       <c r="B64" s="29"/>
       <c r="C64" s="29"/>
@@ -2266,10 +2122,10 @@
       <c r="J64" s="29"/>
       <c r="K64" s="29"/>
       <c r="L64" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="29"/>
       <c r="B65" s="29"/>
       <c r="C65" s="29"/>
@@ -2282,10 +2138,10 @@
       <c r="J65" s="29"/>
       <c r="K65" s="29"/>
       <c r="L65" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="29"/>
       <c r="B66" s="29"/>
       <c r="C66" s="29"/>
@@ -2298,10 +2154,10 @@
       <c r="J66" s="29"/>
       <c r="K66" s="29"/>
       <c r="L66" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="29"/>
       <c r="B67" s="29"/>
       <c r="C67" s="29"/>
@@ -2314,10 +2170,10 @@
       <c r="J67" s="29"/>
       <c r="K67" s="29"/>
       <c r="L67" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="29"/>
       <c r="B68" s="29"/>
       <c r="C68" s="29"/>
@@ -2330,10 +2186,10 @@
       <c r="J68" s="29"/>
       <c r="K68" s="29"/>
       <c r="L68" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="29"/>
       <c r="B69" s="29"/>
       <c r="C69" s="29"/>
@@ -2346,10 +2202,10 @@
       <c r="J69" s="29"/>
       <c r="K69" s="29"/>
       <c r="L69" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="29"/>
       <c r="B70" s="29"/>
       <c r="C70" s="29"/>
@@ -2362,10 +2218,10 @@
       <c r="J70" s="29"/>
       <c r="K70" s="29"/>
       <c r="L70" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="29"/>
       <c r="B71" s="29"/>
       <c r="C71" s="29"/>
@@ -2378,10 +2234,10 @@
       <c r="J71" s="29"/>
       <c r="K71" s="29"/>
       <c r="L71" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="29"/>
       <c r="B72" s="29"/>
       <c r="C72" s="29"/>
@@ -2394,11 +2250,74 @@
       <c r="J72" s="29"/>
       <c r="K72" s="29"/>
       <c r="L72" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="80">
+  <mergeCells count="79">
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="D21:L21"/>
+    <mergeCell ref="D20:L20"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="D18:L18"/>
+    <mergeCell ref="D19:L19"/>
+    <mergeCell ref="L29:L30"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="C26:D27"/>
+    <mergeCell ref="C29:D30"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="L35:L36"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="C32:D33"/>
+    <mergeCell ref="A39:K39"/>
+    <mergeCell ref="A40:K40"/>
+    <mergeCell ref="A41:K41"/>
+    <mergeCell ref="A42:K42"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A49:K49"/>
+    <mergeCell ref="A50:K50"/>
+    <mergeCell ref="A44:K44"/>
+    <mergeCell ref="A45:K45"/>
+    <mergeCell ref="A46:K46"/>
+    <mergeCell ref="A47:K47"/>
+    <mergeCell ref="A48:K48"/>
+    <mergeCell ref="A59:K59"/>
+    <mergeCell ref="A60:K60"/>
+    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="A52:K52"/>
+    <mergeCell ref="A53:K53"/>
+    <mergeCell ref="A54:K54"/>
+    <mergeCell ref="A55:K55"/>
     <mergeCell ref="L13:L14"/>
     <mergeCell ref="A71:K71"/>
     <mergeCell ref="A72:K72"/>
@@ -2415,70 +2334,6 @@
     <mergeCell ref="A56:K56"/>
     <mergeCell ref="A57:K57"/>
     <mergeCell ref="A58:K58"/>
-    <mergeCell ref="A59:K59"/>
-    <mergeCell ref="A60:K60"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="A52:K52"/>
-    <mergeCell ref="A53:K53"/>
-    <mergeCell ref="A54:K54"/>
-    <mergeCell ref="A55:K55"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A49:K49"/>
-    <mergeCell ref="A50:K50"/>
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="A45:K45"/>
-    <mergeCell ref="A46:K46"/>
-    <mergeCell ref="A47:K47"/>
-    <mergeCell ref="A48:K48"/>
-    <mergeCell ref="C35:D36"/>
-    <mergeCell ref="A39:K39"/>
-    <mergeCell ref="A40:K40"/>
-    <mergeCell ref="A41:K41"/>
-    <mergeCell ref="A42:K42"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="L35:L36"/>
-    <mergeCell ref="J35:J36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="C32:D33"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="D18:L18"/>
-    <mergeCell ref="D19:L19"/>
-    <mergeCell ref="L29:L30"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="C26:D27"/>
-    <mergeCell ref="C29:D30"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="D21:L21"/>
-    <mergeCell ref="D20:L20"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="L16:L17"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>